<commit_message>
Added Relay state saving to EEPROM Added MQTT Topic configuration via browser Added defaults values setting while first launching or restoring to defaults
</commit_message>
<xml_diff>
--- a/EEPROM/memory-map.xlsx
+++ b/EEPROM/memory-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>Device Mode</t>
+  </si>
+  <si>
+    <t>Temp Correction</t>
+  </si>
+  <si>
+    <t>Temp Interval</t>
+  </si>
+  <si>
+    <t>MQTT Topic</t>
+  </si>
+  <si>
+    <t>Relay state</t>
   </si>
 </sst>
 </file>
@@ -442,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,188 +518,204 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C5" si="0">D3+1</f>
+        <f t="shared" ref="C4" si="0">D3+1</f>
         <v>104</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D5" si="1">B4+C4-1</f>
+        <f t="shared" ref="D4" si="1">B4+C4-1</f>
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>127</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C6" si="2">D4+1</f>
         <v>105</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
-        <v>231</v>
+        <f t="shared" ref="D5:D8" si="3">B5+C5-1</f>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>32</v>
-      </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C28" si="2">D5+1</f>
-        <v>232</v>
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6" si="3">B6+C6-1</f>
-        <v>263</v>
+        <f t="shared" si="3"/>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="2"/>
-        <v>264</v>
+        <f t="shared" ref="C7:C8" si="4">D6+1</f>
+        <v>118</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D5:D28" si="4">B7+C7-1</f>
-        <v>295</v>
+        <f t="shared" ref="D7" si="5">B7+C7-1</f>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="2"/>
-        <v>296</v>
+        <f t="shared" si="4"/>
+        <v>119</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="4"/>
-        <v>327</v>
+        <f t="shared" si="3"/>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
-        <v>328</v>
+        <f t="shared" ref="C9:C31" si="6">D8+1</f>
+        <v>232</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="4"/>
-        <v>332</v>
+        <f t="shared" ref="D9" si="7">B9+C9-1</f>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>32</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
-        <v>333</v>
+        <f t="shared" si="6"/>
+        <v>264</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="4"/>
-        <v>364</v>
+        <f t="shared" ref="D10:D31" si="8">B10+C10-1</f>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>32</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
-        <v>365</v>
+        <f t="shared" si="6"/>
+        <v>296</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="4"/>
-        <v>396</v>
-      </c>
-      <c r="J11" s="3"/>
+        <f t="shared" si="8"/>
+        <v>327</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="6"/>
+        <v>328</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="8"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="6"/>
+        <v>333</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="8"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="6"/>
+        <v>365</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="8"/>
+        <v>396</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="6"/>
+        <v>397</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="8"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
-        <v>64</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" si="2"/>
-        <v>397</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="4"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
-        <f t="shared" si="2"/>
-        <v>461</v>
-      </c>
-      <c r="D13" s="2">
-        <f t="shared" si="4"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
-        <f t="shared" si="2"/>
-        <v>461</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="4"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <f t="shared" si="2"/>
-        <v>461</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="4"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>32</v>
+      </c>
       <c r="C16" s="2">
-        <f t="shared" si="2"/>
-        <v>461</v>
+        <f t="shared" si="6"/>
+        <v>429</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -695,11 +723,11 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -707,11 +735,11 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -719,11 +747,11 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -731,11 +759,11 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -743,11 +771,11 @@
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -755,11 +783,11 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -767,11 +795,11 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -779,11 +807,11 @@
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -791,11 +819,11 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -803,11 +831,11 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -815,11 +843,11 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>
@@ -827,11 +855,47 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>461</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="8"/>
         <v>460</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OTA done, MQTT done, first firmware released
</commit_message>
<xml_diff>
--- a/EEPROM/memory-map.xlsx
+++ b/EEPROM/memory-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Relay state</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Host Name</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +544,7 @@
         <v>105</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D8" si="3">B5+C5-1</f>
+        <f t="shared" ref="D5:D10" si="3">B5+C5-1</f>
         <v>109</v>
       </c>
     </row>
@@ -566,177 +572,188 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C8" si="4">D6+1</f>
+        <f>D6+1</f>
         <v>118</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7" si="5">B7+C7-1</f>
+        <f t="shared" ref="D7:D10" si="4">B7+C7-1</f>
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>113</v>
-      </c>
       <c r="C8" s="2">
+        <f t="shared" ref="C8:C10" si="5">D7+1</f>
+        <v>119</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="4"/>
-        <v>119</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ref="C9:C31" si="6">D8+1</f>
-        <v>232</v>
+        <f t="shared" si="5"/>
+        <v>125</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9" si="7">B9+C9-1</f>
-        <v>263</v>
+        <f t="shared" si="4"/>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="6"/>
-        <v>264</v>
+        <f t="shared" si="5"/>
+        <v>138</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ref="D10:D31" si="8">B10+C10-1</f>
-        <v>295</v>
+        <f t="shared" si="4"/>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>32</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="6"/>
-        <v>296</v>
+        <f t="shared" ref="C11:C33" si="6">D10+1</f>
+        <v>232</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="8"/>
-        <v>327</v>
+        <f t="shared" ref="D11" si="7">B11+C11-1</f>
+        <v>263</v>
+      </c>
+      <c r="F11">
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="6"/>
-        <v>328</v>
+        <v>264</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="8"/>
-        <v>332</v>
+        <f t="shared" ref="D12:D33" si="8">B12+C12-1</f>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>32</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="6"/>
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="8"/>
-        <v>364</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="6"/>
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="8"/>
-        <v>396</v>
-      </c>
-      <c r="J14" s="3"/>
+        <v>332</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2">
         <v>32</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="6"/>
-        <v>397</v>
+        <v>333</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="8"/>
-        <v>428</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>32</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="6"/>
+        <v>365</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="8"/>
+        <v>396</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="6"/>
+        <v>397</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="8"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="6"/>
         <v>429</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="8"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
-        <f t="shared" si="6"/>
-        <v>461</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="8"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2">
-        <f t="shared" si="6"/>
-        <v>461</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="8"/>
@@ -895,6 +912,30 @@
         <v>461</v>
       </c>
       <c r="D31" s="2">
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="8"/>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="D33" s="2">
         <f t="shared" si="8"/>
         <v>460</v>
       </c>

</xml_diff>

<commit_message>
0.5.2 - defects fixing
</commit_message>
<xml_diff>
--- a/EEPROM/memory-map.xlsx
+++ b/EEPROM/memory-map.xlsx
@@ -472,7 +472,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C13" si="5">D7+1</f>
+        <f t="shared" ref="C8:C12" si="5">D7+1</f>
         <v>119</v>
       </c>
       <c r="D8" s="2">
@@ -677,7 +677,7 @@
         <v>90</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="5"/>
+        <f>D12+1</f>
         <v>142</v>
       </c>
       <c r="D13" s="2">

</xml_diff>